<commit_message>
lci mfh 02 example setup
</commit_message>
<xml_diff>
--- a/model_beef/postprocessing/20230106_final_input_output.xlsx
+++ b/model_beef/postprocessing/20230106_final_input_output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10190" tabRatio="673" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23535" windowHeight="8235" tabRatio="673" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="U Value &amp; Energy demand results" sheetId="1" r:id="rId1"/>
@@ -1192,6 +1192,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1230,24 +1248,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4115,51 +4115,51 @@
       <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="65" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.54296875" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1796875" style="27" customWidth="1"/>
-    <col min="11" max="11" width="21.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.26953125" style="27" customWidth="1"/>
-    <col min="13" max="13" width="16.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.453125" style="27" customWidth="1"/>
-    <col min="15" max="52" width="9.1796875" style="27"/>
+    <col min="1" max="1" width="8.140625" style="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" style="27" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="27" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="27" customWidth="1"/>
+    <col min="15" max="52" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="132"/>
-      <c r="B1" s="132"/>
-      <c r="C1" s="133" t="s">
+    <row r="1" spans="1:52" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="138"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="139" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="129" t="s">
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="131" t="s">
+      <c r="I1" s="137" t="s">
         <v>124</v>
       </c>
-      <c r="J1" s="126" t="s">
+      <c r="J1" s="132" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="128"/>
-    </row>
-    <row r="2" spans="1:52" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="132"/>
-      <c r="B2" s="132"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="134"/>
+    </row>
+    <row r="2" spans="1:52" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="138"/>
+      <c r="B2" s="138"/>
       <c r="C2" s="96" t="s">
         <v>0</v>
       </c>
@@ -4175,8 +4175,8 @@
       <c r="G2" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
       <c r="J2" s="97" t="s">
         <v>117</v>
       </c>
@@ -4231,8 +4231,8 @@
       <c r="AY2" s="99"/>
       <c r="AZ2" s="99"/>
     </row>
-    <row r="3" spans="1:52" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="135" t="s">
+    <row r="3" spans="1:52" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="141" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="66" t="s">
@@ -4263,8 +4263,8 @@
       <c r="M3" s="79"/>
       <c r="N3" s="88"/>
     </row>
-    <row r="4" spans="1:52" s="69" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="136"/>
+    <row r="4" spans="1:52" s="69" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="142"/>
       <c r="B4" s="70" t="s">
         <v>21</v>
       </c>
@@ -4301,8 +4301,8 @@
       </c>
       <c r="N4" s="93"/>
     </row>
-    <row r="5" spans="1:52" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="135" t="s">
+    <row r="5" spans="1:52" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="141" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="66" t="s">
@@ -4335,8 +4335,8 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="6" spans="1:52" s="69" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="136"/>
+    <row r="6" spans="1:52" s="69" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="142"/>
       <c r="B6" s="70" t="s">
         <v>21</v>
       </c>
@@ -4375,8 +4375,8 @@
       </c>
       <c r="N6" s="83"/>
     </row>
-    <row r="7" spans="1:52" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="135" t="s">
+    <row r="7" spans="1:52" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="141" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="66" t="s">
@@ -4407,8 +4407,8 @@
       <c r="M7" s="103"/>
       <c r="N7" s="80"/>
     </row>
-    <row r="8" spans="1:52" s="69" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A8" s="136"/>
+    <row r="8" spans="1:52" s="69" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="142"/>
       <c r="B8" s="70" t="s">
         <v>21</v>
       </c>
@@ -4449,8 +4449,8 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="9" spans="1:52" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="137" t="s">
+    <row r="9" spans="1:52" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="124" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="66" t="s">
@@ -4481,8 +4481,8 @@
       <c r="M9" s="103"/>
       <c r="N9" s="80"/>
     </row>
-    <row r="10" spans="1:52" s="69" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="138"/>
+    <row r="10" spans="1:52" s="69" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="125"/>
       <c r="B10" s="70" t="s">
         <v>21</v>
       </c>
@@ -4519,8 +4519,8 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="11" spans="1:52" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="137" t="s">
+    <row r="11" spans="1:52" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="124" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="66" t="s">
@@ -4551,8 +4551,8 @@
       <c r="M11" s="103"/>
       <c r="N11" s="80"/>
     </row>
-    <row r="12" spans="1:52" s="69" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A12" s="138"/>
+    <row r="12" spans="1:52" s="69" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="125"/>
       <c r="B12" s="70" t="s">
         <v>21</v>
       </c>
@@ -4591,8 +4591,8 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:52" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="141" t="s">
+    <row r="13" spans="1:52" s="49" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="128" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="108" t="s">
@@ -4623,8 +4623,8 @@
       <c r="M13" s="113"/>
       <c r="N13" s="114"/>
     </row>
-    <row r="14" spans="1:52" s="49" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A14" s="142"/>
+    <row r="14" spans="1:52" s="49" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="129"/>
       <c r="B14" s="115" t="s">
         <v>8</v>
       </c>
@@ -4665,8 +4665,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:52" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="137" t="s">
+    <row r="15" spans="1:52" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="124" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="66" t="s">
@@ -4697,8 +4697,8 @@
       <c r="M15" s="103"/>
       <c r="N15" s="80"/>
     </row>
-    <row r="16" spans="1:52" s="69" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="138"/>
+    <row r="16" spans="1:52" s="69" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="125"/>
       <c r="B16" s="70" t="s">
         <v>21</v>
       </c>
@@ -4737,8 +4737,8 @@
       </c>
       <c r="N16" s="83"/>
     </row>
-    <row r="17" spans="1:52" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="137" t="s">
+    <row r="17" spans="1:52" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="124" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="66" t="s">
@@ -4769,8 +4769,8 @@
       <c r="M17" s="103"/>
       <c r="N17" s="80"/>
     </row>
-    <row r="18" spans="1:52" s="69" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A18" s="138"/>
+    <row r="18" spans="1:52" s="69" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="125"/>
       <c r="B18" s="70" t="s">
         <v>21</v>
       </c>
@@ -4811,8 +4811,8 @@
         <v>0.79499999999999993</v>
       </c>
     </row>
-    <row r="19" spans="1:52" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="139" t="s">
+    <row r="19" spans="1:52" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="126" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="60" t="s">
@@ -4881,8 +4881,8 @@
       <c r="AY19" s="27"/>
       <c r="AZ19" s="27"/>
     </row>
-    <row r="20" spans="1:52" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="140"/>
+    <row r="20" spans="1:52" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="127"/>
       <c r="B20" s="62" t="s">
         <v>21</v>
       </c>
@@ -4892,11 +4892,11 @@
       <c r="D20" s="62">
         <v>3203</v>
       </c>
-      <c r="E20" s="124" t="s">
+      <c r="E20" s="130" t="s">
         <v>140</v>
       </c>
-      <c r="F20" s="124"/>
-      <c r="G20" s="125"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="131"/>
       <c r="H20" s="72"/>
       <c r="I20" s="64">
         <v>2.3115541589915846E-4</v>
@@ -4955,8 +4955,8 @@
       <c r="AY20" s="27"/>
       <c r="AZ20" s="27"/>
     </row>
-    <row r="21" spans="1:52" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="137" t="s">
+    <row r="21" spans="1:52" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="124" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="66" t="s">
@@ -4987,8 +4987,8 @@
       <c r="M21" s="103"/>
       <c r="N21" s="80"/>
     </row>
-    <row r="22" spans="1:52" s="69" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A22" s="138"/>
+    <row r="22" spans="1:52" s="69" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="125"/>
       <c r="B22" s="70" t="s">
         <v>21</v>
       </c>
@@ -5027,8 +5027,8 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:52" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="137" t="s">
+    <row r="23" spans="1:52" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="124" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="66" t="s">
@@ -5059,8 +5059,8 @@
       <c r="M23" s="103"/>
       <c r="N23" s="80"/>
     </row>
-    <row r="24" spans="1:52" s="69" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A24" s="138"/>
+    <row r="24" spans="1:52" s="69" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="125"/>
       <c r="B24" s="70" t="s">
         <v>21</v>
       </c>
@@ -5101,8 +5101,8 @@
         <v>1.3466666666666667</v>
       </c>
     </row>
-    <row r="25" spans="1:52" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="139" t="s">
+    <row r="25" spans="1:52" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="126" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="60" t="s">
@@ -5171,8 +5171,8 @@
       <c r="AY25" s="27"/>
       <c r="AZ25" s="27"/>
     </row>
-    <row r="26" spans="1:52" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A26" s="140"/>
+    <row r="26" spans="1:52" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="127"/>
       <c r="B26" s="62" t="s">
         <v>21</v>
       </c>
@@ -5251,89 +5251,81 @@
       <c r="AY26" s="27"/>
       <c r="AZ26" s="27"/>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
       <c r="I29" s="27"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>0.38966822533956802</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>1.4416146083613647E-4</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>7.8933043004899298E-2</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>0.26548672566371684</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="27">
         <v>0.27027027027027029</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="27"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="27">
         <v>7.317073170731707E-5</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="27"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="27">
         <v>2.3115541589915846E-4</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="27"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="27"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="27"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="27">
         <v>0.57991513437057995</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="27"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="27">
         <v>8.516436722875149E-5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="H1:H2"/>
@@ -5344,6 +5336,14 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5357,31 +5357,31 @@
   </sheetPr>
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.26953125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="95"/>
       <c r="B6" s="95" t="s">
         <v>130</v>
@@ -5396,7 +5396,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="95" t="s">
         <v>23</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>80.59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="95" t="s">
         <v>24</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>230.77</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="95" t="s">
         <v>25</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>104.76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="95" t="s">
         <v>26</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>177.36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="95" t="s">
         <v>27</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>68.55</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="95" t="s">
         <v>29</v>
       </c>
@@ -5492,7 +5492,7 @@
         <v>42.61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="95" t="s">
         <v>30</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>119.39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="95" t="s">
         <v>32</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>159.12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="95" t="s">
         <v>33</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>170.87</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="95" t="s">
         <v>34</v>
       </c>
@@ -5553,14 +5553,14 @@
         <v>107.83</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="122"/>
       <c r="B17" s="122"/>
       <c r="C17" s="122"/>
       <c r="D17" s="122"/>
       <c r="E17" s="122"/>
     </row>
-    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="95"/>
       <c r="B18" s="95" t="s">
         <v>130</v>
@@ -5575,7 +5575,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="95" t="s">
         <v>23</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>1.3431666666666666</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="95" t="s">
         <v>24</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>3.846166666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="95" t="s">
         <v>25</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>1.746</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="95" t="s">
         <v>26</v>
       </c>
@@ -5659,7 +5659,7 @@
         <v>2.9560000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="95" t="s">
         <v>27</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>1.1424999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="95" t="s">
         <v>29</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>0.71016666666666661</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="95" t="s">
         <v>30</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>1.9898333333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="95" t="s">
         <v>32</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>2.6520000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="95" t="s">
         <v>33</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>2.8478333333333334</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="95" t="s">
         <v>34</v>
       </c>
@@ -5785,9 +5785,9 @@
         <v>1.7971666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -5823,7 +5823,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>9.3388429752066029E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>0.35250000000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>0.18163580246913577</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>0.59245283018867934</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>0.41585714285714287</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>6.6154754873006746E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>2.2627118644067801E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>1.3958333333333364E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>0.43679487179487192</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>0.33913043478260868</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I45" t="s">
         <v>33</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>6.0365217391304347</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>1.4014234875444833</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>84.77</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -6384,7 +6384,7 @@
       <c r="K48" s="49"/>
       <c r="L48" s="49"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -6416,7 +6416,7 @@
       <c r="R49" s="49"/>
       <c r="S49" s="49"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>27</v>
       </c>
@@ -6448,7 +6448,7 @@
       <c r="R50" s="49"/>
       <c r="S50" s="49"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -6480,7 +6480,7 @@
       <c r="R51" s="49"/>
       <c r="S51" s="49"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -6512,7 +6512,7 @@
       <c r="R52" s="49"/>
       <c r="S52" s="49"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>33</v>
       </c>
@@ -6544,7 +6544,7 @@
       <c r="R53" s="49"/>
       <c r="S53" s="49"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>30</v>
       </c>
@@ -6576,7 +6576,7 @@
       <c r="R54" s="49"/>
       <c r="S54" s="49"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -6608,7 +6608,7 @@
       <c r="R55" s="49"/>
       <c r="S55" s="49"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>23</v>
       </c>
@@ -6640,7 +6640,7 @@
       <c r="R56" s="49"/>
       <c r="S56" s="49"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -6672,7 +6672,7 @@
       <c r="R57" s="49"/>
       <c r="S57" s="49"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>28</v>
       </c>
@@ -6704,7 +6704,7 @@
       <c r="R58" s="49"/>
       <c r="S58" s="49"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H59" s="49"/>
       <c r="I59" s="49"/>
       <c r="J59" s="49"/>
@@ -6718,7 +6718,7 @@
       <c r="R59" s="49"/>
       <c r="S59" s="49"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H60" s="49"/>
       <c r="I60" s="49"/>
       <c r="J60" s="49"/>
@@ -6732,7 +6732,7 @@
       <c r="R60" s="49"/>
       <c r="S60" s="49"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H61" s="49"/>
       <c r="I61" s="49"/>
       <c r="J61" s="49"/>
@@ -6746,7 +6746,7 @@
       <c r="R61" s="49"/>
       <c r="S61" s="49"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H62" s="49"/>
       <c r="I62" s="49"/>
       <c r="J62" s="49"/>
@@ -6760,7 +6760,7 @@
       <c r="R62" s="49"/>
       <c r="S62" s="49"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H63" s="49"/>
       <c r="I63" s="49"/>
       <c r="J63" s="49"/>
@@ -6774,7 +6774,7 @@
       <c r="R63" s="49"/>
       <c r="S63" s="49"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H64" s="49"/>
       <c r="I64" s="49"/>
       <c r="J64" s="49"/>
@@ -6788,7 +6788,7 @@
       <c r="R64" s="49"/>
       <c r="S64" s="49"/>
     </row>
-    <row r="65" spans="8:19" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H65" s="49"/>
       <c r="I65" s="49"/>
       <c r="J65" s="49"/>
@@ -6802,7 +6802,7 @@
       <c r="R65" s="49"/>
       <c r="S65" s="49"/>
     </row>
-    <row r="66" spans="8:19" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H66" s="49"/>
       <c r="I66" s="49"/>
       <c r="J66" s="49"/>
@@ -6816,7 +6816,7 @@
       <c r="R66" s="49"/>
       <c r="S66" s="49"/>
     </row>
-    <row r="67" spans="8:19" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H67" s="49"/>
       <c r="I67" s="49"/>
       <c r="J67" s="49"/>
@@ -6830,7 +6830,7 @@
       <c r="R67" s="49"/>
       <c r="S67" s="49"/>
     </row>
-    <row r="68" spans="8:19" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H68" s="49"/>
       <c r="I68" s="49"/>
       <c r="J68" s="49"/>
@@ -6844,7 +6844,7 @@
       <c r="R68" s="49"/>
       <c r="S68" s="49"/>
     </row>
-    <row r="69" spans="8:19" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H69" s="49"/>
       <c r="I69" s="49"/>
       <c r="J69" s="49"/>
@@ -6871,18 +6871,18 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="90.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>54</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>56</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>57</v>
       </c>
@@ -6906,52 +6906,52 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>67</v>
       </c>
@@ -6983,24 +6983,24 @@
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="10"/>
-    <col min="2" max="2" width="15.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" style="10" customWidth="1"/>
-    <col min="4" max="5" width="11.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="10"/>
+    <col min="2" max="2" width="15.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="10" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="10" customWidth="1"/>
     <col min="11" max="15" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="20.81640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.453125" style="26" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7265625" style="10"/>
+    <col min="16" max="16" width="20.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
         <v>73</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11" t="s">
         <v>75</v>
@@ -7070,7 +7070,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
@@ -7105,7 +7105,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
@@ -7142,7 +7142,7 @@
       </c>
       <c r="P4" s="22"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
@@ -7180,7 +7180,7 @@
       <c r="P5" s="22"/>
       <c r="Q5" s="12"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>26</v>
       </c>
@@ -7225,7 +7225,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
@@ -7267,7 +7267,7 @@
       <c r="P7" s="22"/>
       <c r="Q7" s="12"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
@@ -7305,7 +7305,7 @@
       <c r="P8" s="22"/>
       <c r="Q8" s="12"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>30</v>
       </c>
@@ -7389,7 +7389,7 @@
       <c r="P10" s="22"/>
       <c r="Q10" s="12"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>31</v>
       </c>
@@ -7439,7 +7439,7 @@
       <c r="P11" s="22"/>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>32</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>33</v>
       </c>
@@ -7545,7 +7545,7 @@
       <c r="P13" s="22"/>
       <c r="Q13" s="12"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>34</v>
       </c>
@@ -7595,7 +7595,7 @@
       <c r="P14" s="22"/>
       <c r="Q14" s="12"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -7611,7 +7611,7 @@
       <c r="Q20" s="12"/>
       <c r="R20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -7627,7 +7627,7 @@
       <c r="Q21" s="12"/>
       <c r="R21" s="8"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -7643,7 +7643,7 @@
       <c r="Q22" s="12"/>
       <c r="R22" s="8"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="G23" s="8"/>
       <c r="I23" s="8"/>
@@ -7652,7 +7652,7 @@
       <c r="L23" s="8"/>
       <c r="R23" s="8"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -7663,7 +7663,7 @@
       <c r="L24" s="8"/>
       <c r="R24" s="12"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="G25" s="12"/>
       <c r="I25" s="12"/>
@@ -7672,20 +7672,20 @@
       <c r="P25" s="24"/>
       <c r="Q25" s="32"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -7709,24 +7709,24 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="49"/>
-    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="49"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="49" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="49" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="57" t="s">
         <v>103</v>
       </c>
@@ -7750,7 +7750,7 @@
       </c>
       <c r="M2" s="27"/>
     </row>
-    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="58"/>
       <c r="C3" s="52"/>
       <c r="D3" s="42" t="s">
@@ -7776,7 +7776,7 @@
       <c r="L3" s="151"/>
       <c r="M3" s="27"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>29</v>
       </c>
@@ -7806,7 +7806,7 @@
       </c>
       <c r="M4" s="27"/>
     </row>
-    <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="38" t="s">
         <v>32</v>
       </c>
@@ -7839,8 +7839,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:13" s="49" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="44" t="s">
         <v>101</v>
       </c>
@@ -7858,7 +7858,7 @@
       <c r="J7" s="49"/>
       <c r="L7" s="27"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="36" t="s">
         <v>29</v>
       </c>
@@ -7875,7 +7875,7 @@
       <c r="I8" s="49"/>
       <c r="J8" s="49"/>
     </row>
-    <row r="9" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="38" t="s">
         <v>32</v>
       </c>
@@ -7892,12 +7892,12 @@
       <c r="I9" s="49"/>
       <c r="J9" s="49"/>
     </row>
-    <row r="10" spans="2:13" s="49" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
     </row>
-    <row r="12" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="59"/>
       <c r="C12" s="59" t="s">
         <v>108</v>
@@ -7912,7 +7912,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="59" t="s">
         <v>29</v>
       </c>
@@ -7929,7 +7929,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="59" t="s">
         <v>32</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>0.46800000000000003</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="36" t="s">
         <v>23</v>
       </c>
@@ -7976,7 +7976,7 @@
       </c>
       <c r="M17" s="27"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="36" t="s">
         <v>26</v>
       </c>

</xml_diff>